<commit_message>
nhúng sidebar cho admin #50
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\testGitHub\Test\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F3EC39-BC94-4113-B81D-F0F0955DB414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267CB50B-B3AA-4AFF-B98C-1698CCE65650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timeline" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">timeline!$H$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1166,6 +1169,7 @@
       <formula1>"Hoàn Thành, Đang Thực Hiện, Dự Kiến"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>